<commit_message>
Modified the test file
</commit_message>
<xml_diff>
--- a/EmployeesInformations.xlsx
+++ b/EmployeesInformations.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26006"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="483" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EE39D66-A830-4BD3-8724-3AFDA3A2E3DB}"/>
+  <xr:revisionPtr revIDLastSave="488" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F576E80-373C-4BE1-BE78-B2BCDF994607}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Employees" sheetId="1" r:id="rId1"/>
+    <sheet name="Managers" sheetId="2" r:id="rId2"/>
+    <sheet name="Mentors" sheetId="3" r:id="rId3"/>
+    <sheet name="UsefulLinks" sheetId="4" r:id="rId4"/>
+    <sheet name="PracticeFormular" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>

</xml_diff>